<commit_message>
Improvements to Decouplers #39
</commit_message>
<xml_diff>
--- a/Source/CalcsAndModels/StockParts.xlsx
+++ b/Source/CalcsAndModels/StockParts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="4080" windowWidth="30840" windowHeight="18975"/>
+    <workbookView xWindow="3765" yWindow="4080" windowWidth="30840" windowHeight="18975" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tanks" sheetId="3" r:id="rId1"/>
@@ -65,8 +65,170 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Chris Wood</author>
+  </authors>
+  <commentList>
+    <comment ref="P1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chris Wood:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The best fit does make some reasonable physical sense. The mass of the explosives is minimal (for anything with an ISP better than a fart in a jar) so make the mass proportional to the area. 
+This treats all the stock parts as essentially the same length.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chris Wood:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+I tried a few models here. You'd expect the max to go up on the square, but you rapidly enter the realm of ridiculous impulses. 
+This way gives us sensible results.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chris Wood:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+SO this trial of fit calculated the mass as proportional to the cube of the diameter. 
+This would be the case if the length of the part was a fixed ratio to the width (ie: aspect ratio as per nosecones).
+It's not a great fit, big variance from stock</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chris Wood:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+I really had high hopes for this equation.
+It makes sense - the mass is proportional to the area of the decoupler, plus some mass for the impulse force. If it's a separator then then the decoupler mass is doubled.
+The problem is the fit gets worse the more one uses the impulse, plus the specific impuse I calculated would be terrible compared to any known fuel.
+The stdev is the worst of the lot.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AF1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chris Wood:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The old way - mass is proportional to volume.
+Unfortunatly since there's no consistency in the stock densities this gives a pretty bad fit.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chris Wood:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Our decouplers are 0.2 long, so this is the density if the stock decouplers were also 0.2 long.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="167">
   <si>
     <t>dia</t>
   </si>
@@ -425,9 +587,6 @@
     <t>area</t>
   </si>
   <si>
-    <t>force/area</t>
-  </si>
-  <si>
     <t>WetMass</t>
   </si>
   <si>
@@ -504,13 +663,79 @@
   </si>
   <si>
     <t>fuelTank3-2</t>
+  </si>
+  <si>
+    <t>mass/area</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>size3Decoupler</t>
+  </si>
+  <si>
+    <t>m/force</t>
+  </si>
+  <si>
+    <t>mass/area/aparatus</t>
+  </si>
+  <si>
+    <t>sides</t>
+  </si>
+  <si>
+    <t>m/aparatus</t>
+  </si>
+  <si>
+    <t>calc mass</t>
+  </si>
+  <si>
+    <t>Fit</t>
+  </si>
+  <si>
+    <t>fit</t>
+  </si>
+  <si>
+    <t>Failed! Mass = dens * vol</t>
+  </si>
+  <si>
+    <t>mass = c * area</t>
+  </si>
+  <si>
+    <t>Failed! Mass = c1 * area * ends + c2 * force</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>StDev</t>
+  </si>
+  <si>
+    <t>max Force = c * dia</t>
+  </si>
+  <si>
+    <t>Impulse</t>
+  </si>
+  <si>
+    <t>mass/dia^3</t>
+  </si>
+  <si>
+    <t>Failed: mass = c * dia^3 (ie: fixed aspect ratio)</t>
+  </si>
+  <si>
+    <t>vol*av dens</t>
+  </si>
+  <si>
+    <t>maxForce</t>
+  </si>
+  <si>
+    <t>impulse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -582,6 +807,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -600,7 +839,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -626,19 +865,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="25" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -664,6 +907,7 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="25" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -957,8 +1201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -971,19 +1215,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="N1" s="6" t="s">
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="N1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="6"/>
+      <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:28">
       <c r="B2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -995,7 +1239,7 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I2" t="s">
         <v>16</v>
@@ -1600,7 +1844,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C12">
         <v>2.5</v>
@@ -1676,7 +1920,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C13">
         <v>2.5</v>
@@ -1749,10 +1993,10 @@
     </row>
     <row r="14" spans="1:28">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C14">
         <v>3.75</v>
@@ -1828,10 +2072,10 @@
     </row>
     <row r="15" spans="1:28">
       <c r="A15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C15">
         <v>3.75</v>
@@ -1907,10 +2151,10 @@
     </row>
     <row r="16" spans="1:28">
       <c r="A16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C16">
         <v>3.75</v>
@@ -2369,19 +2613,19 @@
     </row>
     <row r="32" spans="1:28">
       <c r="A32" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B32" s="1"/>
       <c r="G32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:28">
       <c r="A33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" t="s">
         <v>127</v>
-      </c>
-      <c r="B33" t="s">
-        <v>128</v>
       </c>
       <c r="C33">
         <v>0.625</v>
@@ -2397,7 +2641,7 @@
         <v>700</v>
       </c>
       <c r="I33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J33">
         <v>0.2</v>
@@ -2436,10 +2680,10 @@
     </row>
     <row r="34" spans="1:28">
       <c r="A34" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" t="s">
         <v>132</v>
-      </c>
-      <c r="B34" t="s">
-        <v>133</v>
       </c>
       <c r="E34">
         <v>0.05</v>
@@ -2465,10 +2709,10 @@
     </row>
     <row r="35" spans="1:28">
       <c r="A35" t="s">
+        <v>129</v>
+      </c>
+      <c r="B35" t="s">
         <v>130</v>
-      </c>
-      <c r="B35" t="s">
-        <v>131</v>
       </c>
       <c r="C35">
         <v>0.3</v>
@@ -2483,7 +2727,7 @@
         <v>400</v>
       </c>
       <c r="I35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J35">
         <v>0.2</v>
@@ -2529,10 +2773,10 @@
         <v>57</v>
       </c>
       <c r="Z37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AA37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:28">
@@ -2686,10 +2930,10 @@
     </row>
     <row r="40" spans="1:28">
       <c r="A40" t="s">
+        <v>140</v>
+      </c>
+      <c r="B40" t="s">
         <v>141</v>
-      </c>
-      <c r="B40" t="s">
-        <v>142</v>
       </c>
       <c r="C40">
         <v>1.25</v>
@@ -2846,7 +3090,7 @@
     </row>
     <row r="43" spans="1:28">
       <c r="A43" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B43" s="1"/>
       <c r="G43" t="s">
@@ -2859,10 +3103,10 @@
         <v>57</v>
       </c>
       <c r="Z43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AA43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:28">
@@ -3106,302 +3350,870 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.85546875" style="6"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="B1" t="s">
+    <row r="1" spans="1:33">
+      <c r="P1" t="s">
+        <v>156</v>
+      </c>
+      <c r="S1" t="s">
+        <v>160</v>
+      </c>
+      <c r="W1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33">
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C2" t="s">
         <v>59</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G2" t="s">
         <v>54</v>
       </c>
-      <c r="E1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I2" t="s">
         <v>60</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L2" t="s">
         <v>4</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M2" t="s">
         <v>68</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N2" t="s">
         <v>118</v>
       </c>
-      <c r="M1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" t="s">
+      <c r="P2" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="S2" t="s">
+        <v>165</v>
+      </c>
+      <c r="T2" t="s">
+        <v>166</v>
+      </c>
+      <c r="W2" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>149</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>152</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>164</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
+      <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3">
+        <f>0.07590994+0.07590994</f>
+        <v>0.15181987999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.625</v>
+      </c>
+      <c r="E3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <f>G3*0.02</f>
+        <v>0.3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3">
+        <f>2*PI()*(D3/2)*C3</f>
+        <v>0.29809763729805244</v>
+      </c>
+      <c r="M3">
+        <f>E3/L3</f>
+        <v>5.031908382756578E-2</v>
+      </c>
+      <c r="N3">
+        <f>PI()*(D3/2)^2</f>
+        <v>0.30679615757712825</v>
+      </c>
+      <c r="P3">
+        <f>E3/N3</f>
+        <v>4.8892398517830248E-2</v>
+      </c>
+      <c r="Q3" s="6">
+        <f>P3/P$12</f>
+        <v>0.7415399705738106</v>
+      </c>
+      <c r="S3">
+        <f>S$12*D3</f>
+        <v>250</v>
+      </c>
+      <c r="T3">
+        <f>S3*0.02</f>
+        <v>5</v>
+      </c>
+      <c r="U3" s="6">
+        <f>G3/S3</f>
+        <v>0.06</v>
+      </c>
+      <c r="W3">
+        <f>E3/D3^3</f>
+        <v>6.1439999999999995E-2</v>
+      </c>
+      <c r="X3" s="6">
+        <f>W3/W$12</f>
+        <v>1.5530257639304974</v>
+      </c>
+      <c r="Z3">
+        <f>G3*Z$12</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="AA3">
+        <f>(E3-Z3)/F3</f>
+        <v>1.35E-2</v>
+      </c>
+      <c r="AB3">
+        <f>AA3/N3</f>
+        <v>4.4003158666047225E-2</v>
+      </c>
+      <c r="AC3">
+        <f>N3*AB$12*F3+G3*Z$12</f>
+        <v>1.4759920634920634E-2</v>
+      </c>
+      <c r="AD3" s="6">
+        <f>AC3/E3</f>
+        <v>0.98399470899470898</v>
+      </c>
+      <c r="AF3">
+        <f>L3*M$12</f>
+        <v>1.8590066827907779E-2</v>
+      </c>
+      <c r="AG3" s="6">
+        <f>AF3/E3</f>
+        <v>1.2393377885271852</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33">
+      <c r="A4" t="s">
         <v>58</v>
       </c>
-      <c r="B2">
+      <c r="C4">
         <f>0.0650517+0.1329949</f>
         <v>0.19804660000000002</v>
       </c>
-      <c r="C2">
+      <c r="D4">
         <v>1.25</v>
       </c>
-      <c r="D2">
+      <c r="E4">
+        <v>0.05</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
         <v>250</v>
       </c>
-      <c r="E2">
-        <v>0.05</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="H4">
+        <f t="shared" ref="H4:H6" si="0">G4*0.02</f>
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
         <v>18</v>
       </c>
-      <c r="I2">
-        <f t="shared" ref="I2:I8" si="0">2*PI()*(C2/2)*B2</f>
+      <c r="L4">
+        <f>2*PI()*(D4/2)*C4</f>
         <v>0.77772717953554549</v>
       </c>
-      <c r="J2">
-        <f t="shared" ref="J2:J8" si="1">E2/I2</f>
+      <c r="M4">
+        <f>E4/L4</f>
         <v>6.4289896657411069E-2</v>
       </c>
-      <c r="L2">
-        <f>PI()*(C2/2)^2</f>
+      <c r="N4">
+        <f>PI()*(D4/2)^2</f>
         <v>1.227184630308513</v>
       </c>
-      <c r="M2">
-        <f>D2/L2</f>
-        <v>203.71832715762602</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3">
-        <f>0.07590994+0.07590994</f>
-        <v>0.15181987999999999</v>
-      </c>
-      <c r="C3">
-        <v>0.625</v>
-      </c>
-      <c r="D3">
-        <v>15</v>
-      </c>
-      <c r="E3">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3">
-        <f>2*PI()*(C3/2)*B3</f>
-        <v>0.29809763729805244</v>
-      </c>
-      <c r="J3">
-        <f>E3/I3</f>
-        <v>5.031908382756578E-2</v>
-      </c>
-      <c r="L3">
-        <f>PI()*(C3/2)^2</f>
-        <v>0.30679615757712825</v>
-      </c>
-      <c r="M3">
-        <f>D3/L3</f>
-        <v>48.892398517830244</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" t="s">
+      <c r="P4">
+        <f>E4/N4</f>
+        <v>4.074366543152521E-2</v>
+      </c>
+      <c r="Q4" s="6">
+        <f>P4/P$12</f>
+        <v>0.61794997547817554</v>
+      </c>
+      <c r="S4">
+        <f>S$12*D4</f>
+        <v>500</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ref="T4:T10" si="1">S4*0.02</f>
+        <v>10</v>
+      </c>
+      <c r="U4" s="6">
+        <f>G4/S4</f>
+        <v>0.5</v>
+      </c>
+      <c r="W4">
+        <f>E4/D4^3</f>
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="X4" s="6">
+        <f>W4/W$12</f>
+        <v>0.64709406830437399</v>
+      </c>
+      <c r="Z4">
+        <f>G4*Z$12</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AA4">
+        <f>(E4-Z4)/F4</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AB4">
+        <f>AA4/N4</f>
+        <v>2.0371832715762605E-2</v>
+      </c>
+      <c r="AC4">
+        <f>N4*AB$12*F4+G4*Z$12</f>
+        <v>7.8039682539682548E-2</v>
+      </c>
+      <c r="AD4" s="6">
+        <f>AC4/E4</f>
+        <v>1.5607936507936508</v>
+      </c>
+      <c r="AF4">
+        <f t="shared" ref="AF4:AF10" si="2">L4*M$12</f>
+        <v>4.8500888408552573E-2</v>
+      </c>
+      <c r="AG4" s="6">
+        <f>AF4/E4</f>
+        <v>0.97001776817105145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33">
+      <c r="A5" t="s">
         <v>63</v>
       </c>
-      <c r="B4">
+      <c r="C5">
         <f>0.4508572+0.3654699</f>
         <v>0.81632710000000008</v>
       </c>
-      <c r="C4">
+      <c r="D5">
         <v>2.5</v>
       </c>
-      <c r="D4">
+      <c r="E5">
+        <v>0.4</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
         <v>250</v>
       </c>
-      <c r="E4">
-        <v>0.4</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
         <v>23</v>
       </c>
-      <c r="I4">
-        <f>2*PI()*(C4/2)*B4</f>
+      <c r="L5">
+        <f>2*PI()*(D5/2)*C5</f>
         <v>6.4114180507156515</v>
       </c>
-      <c r="J4">
-        <f>E4/I4</f>
+      <c r="M5">
+        <f>E5/L5</f>
         <v>6.2388694175908782E-2</v>
       </c>
-      <c r="L4">
-        <f>PI()*(C4/2)^2</f>
+      <c r="N5">
+        <f>PI()*(D5/2)^2</f>
         <v>4.908738521234052</v>
       </c>
-      <c r="M4">
-        <f>D4/L4</f>
-        <v>50.929581789406505</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B5">
+      <c r="P5">
+        <f>E5/N5</f>
+        <v>8.148733086305042E-2</v>
+      </c>
+      <c r="Q5" s="6">
+        <f>P5/P$12</f>
+        <v>1.2358999509563511</v>
+      </c>
+      <c r="S5">
+        <f>S$12*D5</f>
+        <v>1000</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="U5" s="6">
+        <f>G5/S5</f>
+        <v>0.25</v>
+      </c>
+      <c r="W5">
+        <f>E5/D5^3</f>
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="X5" s="6">
+        <f>W5/W$12</f>
+        <v>0.64709406830437399</v>
+      </c>
+      <c r="Z5">
+        <f>G5*Z$12</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AA5">
+        <f>(E5-Z5)/F5</f>
+        <v>0.375</v>
+      </c>
+      <c r="AB5">
+        <f>AA5/N5</f>
+        <v>7.6394372684109757E-2</v>
+      </c>
+      <c r="AC5">
+        <f>N5*AB$12*F5+G5*Z$12</f>
+        <v>0.23715873015873015</v>
+      </c>
+      <c r="AD5" s="6">
+        <f>AC5/E5</f>
+        <v>0.59289682539682531</v>
+      </c>
+      <c r="AF5">
+        <f t="shared" si="2"/>
+        <v>0.39983104564256433</v>
+      </c>
+      <c r="AG5" s="6">
+        <f>AF5/E5</f>
+        <v>0.99957761410641077</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33">
+      <c r="A6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6">
         <v>0.87070789999999998</v>
       </c>
-      <c r="C5">
+      <c r="D6">
         <v>3.75</v>
       </c>
-      <c r="D5">
+      <c r="E6">
+        <v>0.8</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
         <v>100</v>
       </c>
-      <c r="E5">
-        <v>0.8</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="H6">
+        <f>G6*0.02</f>
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
         <v>22</v>
       </c>
-      <c r="I5">
-        <f>2*PI()*(C5/2)*B5</f>
+      <c r="L6">
+        <f>2*PI()*(D6/2)*C6</f>
         <v>10.257785782734734</v>
       </c>
-      <c r="J5">
-        <f>E5/I5</f>
+      <c r="M6">
+        <f>E6/L6</f>
         <v>7.7989540525062462E-2</v>
       </c>
-      <c r="L5">
-        <f>PI()*(C5/2)^2</f>
+      <c r="N6">
+        <f>PI()*(D6/2)^2</f>
         <v>11.044661672776616</v>
       </c>
-      <c r="M5">
-        <f>D5/L5</f>
-        <v>9.0541478736722691</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" t="s">
+      <c r="P6">
+        <f>E6/N6</f>
+        <v>7.2433182989378148E-2</v>
+      </c>
+      <c r="Q6" s="6">
+        <f>P6/P$12</f>
+        <v>1.0985777341834231</v>
+      </c>
+      <c r="S6">
+        <f>S$12*D6</f>
+        <v>1500</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="U6" s="6">
+        <f>G6/S6</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="W6">
+        <f>E6/D6^3</f>
+        <v>1.5170370370370371E-2</v>
+      </c>
+      <c r="X6" s="6">
+        <f>W6/W$12</f>
+        <v>0.38346315158777716</v>
+      </c>
+      <c r="Z6">
+        <f>G6*Z$12</f>
+        <v>0.01</v>
+      </c>
+      <c r="AA6">
+        <f>(E6-Z6)/F6</f>
+        <v>0.79</v>
+      </c>
+      <c r="AB6">
+        <f>AA6/N6</f>
+        <v>7.1527768202010927E-2</v>
+      </c>
+      <c r="AC6">
+        <f>N6*AB$12*F6+G6*Z$12</f>
+        <v>0.48735714285714288</v>
+      </c>
+      <c r="AD6" s="6">
+        <f>AC6/E6</f>
+        <v>0.60919642857142853</v>
+      </c>
+      <c r="AF6">
+        <f t="shared" si="2"/>
+        <v>0.63969954587978506</v>
+      </c>
+      <c r="AG6" s="6">
+        <f>AF6/E6</f>
+        <v>0.79962443234973124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33">
+      <c r="U7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AG7" s="6"/>
+    </row>
+    <row r="8" spans="1:33">
+      <c r="A8" t="s">
         <v>66</v>
       </c>
-      <c r="B7">
+      <c r="C8">
         <f>0.07590994*2</f>
         <v>0.15181987999999999</v>
       </c>
-      <c r="C7">
+      <c r="D8">
         <v>0.625</v>
       </c>
-      <c r="D7">
+      <c r="E8">
+        <v>0.02</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
         <v>15</v>
       </c>
-      <c r="E7">
-        <v>0.02</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="H8">
+        <f t="shared" ref="H8:H10" si="3">G8*0.02</f>
+        <v>0.3</v>
+      </c>
+      <c r="I8" t="s">
         <v>65</v>
       </c>
-      <c r="I7">
-        <f>2*PI()*(C7/2)*B7</f>
+      <c r="L8">
+        <f>2*PI()*(D8/2)*C8</f>
         <v>0.29809763729805244</v>
       </c>
-      <c r="J7">
-        <f>E7/I7</f>
+      <c r="M8">
+        <f>E8/L8</f>
         <v>6.7092111770087712E-2</v>
       </c>
-      <c r="L7">
-        <f>PI()*(C7/2)^2</f>
+      <c r="N8">
+        <f>PI()*(D8/2)^2</f>
         <v>0.30679615757712825</v>
       </c>
-      <c r="M7">
-        <f>D7/L7</f>
-        <v>48.892398517830244</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" t="s">
+      <c r="P8">
+        <f>E8/N8</f>
+        <v>6.518986469044033E-2</v>
+      </c>
+      <c r="Q8" s="6">
+        <f>P8/P$12</f>
+        <v>0.98871996076508084</v>
+      </c>
+      <c r="S8">
+        <f>S$12*D8</f>
+        <v>250</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="U8" s="6">
+        <f>G8/S8</f>
+        <v>0.06</v>
+      </c>
+      <c r="W8">
+        <f>E8/D8^3</f>
+        <v>8.1920000000000007E-2</v>
+      </c>
+      <c r="X8" s="6">
+        <f>W8/W$12</f>
+        <v>2.0707010185739967</v>
+      </c>
+      <c r="Z8">
+        <f>G8*Z$12</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="AA8">
+        <f>(E8-Z8)/F8</f>
+        <v>9.2499999999999995E-3</v>
+      </c>
+      <c r="AB8">
+        <f>AA8/N8</f>
+        <v>3.015031241932865E-2</v>
+      </c>
+      <c r="AC8">
+        <f>N8*AB$12*F8+G8*Z$12</f>
+        <v>2.8019841269841271E-2</v>
+      </c>
+      <c r="AD8" s="6">
+        <f>AC8/E8</f>
+        <v>1.4009920634920636</v>
+      </c>
+      <c r="AF8">
+        <f t="shared" si="2"/>
+        <v>1.8590066827907779E-2</v>
+      </c>
+      <c r="AG8" s="6">
+        <f>AF8/E8</f>
+        <v>0.92950334139538893</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33">
+      <c r="A9" t="s">
         <v>62</v>
       </c>
-      <c r="B8">
+      <c r="C9">
         <f>0.1833064*2</f>
         <v>0.36661280000000002</v>
       </c>
-      <c r="C8">
+      <c r="D9">
         <v>1.25</v>
       </c>
-      <c r="D8">
+      <c r="E9">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
         <v>250</v>
       </c>
-      <c r="E8">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
         <v>65</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
+      <c r="L9">
+        <f t="shared" ref="L9" si="4">2*PI()*(D9/2)*C9</f>
         <v>1.4396850989899801</v>
       </c>
-      <c r="J8">
+      <c r="M9">
+        <f>E9/L9</f>
+        <v>5.2094725473380746E-2</v>
+      </c>
+      <c r="N9">
+        <f>PI()*(D9/2)^2</f>
+        <v>1.227184630308513</v>
+      </c>
+      <c r="P9">
+        <f>E9/N9</f>
+        <v>6.1115498147287804E-2</v>
+      </c>
+      <c r="Q9" s="6">
+        <f>P9/P$12</f>
+        <v>0.92692496321726314</v>
+      </c>
+      <c r="S9">
+        <f>S$12*D9</f>
+        <v>500</v>
+      </c>
+      <c r="T9">
         <f t="shared" si="1"/>
-        <v>5.2094725473380746E-2</v>
-      </c>
-      <c r="L8">
-        <f t="shared" ref="L8" si="2">PI()*(C8/2)^2</f>
-        <v>1.227184630308513</v>
-      </c>
-      <c r="M8">
-        <f t="shared" ref="M8" si="3">D8/L8</f>
-        <v>203.71832715762602</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="U9" s="6">
+        <f>G9/S9</f>
+        <v>0.5</v>
+      </c>
+      <c r="W9">
+        <f>E9/D9^3</f>
+        <v>3.8399999999999997E-2</v>
+      </c>
+      <c r="X9" s="6">
+        <f>W9/W$12</f>
+        <v>0.97064110245656088</v>
+      </c>
+      <c r="Z9">
+        <f>G9*Z$12</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AA9">
+        <f>(E9-Z9)/F9</f>
+        <v>2.4999999999999998E-2</v>
+      </c>
+      <c r="AB9">
+        <f>AA9/N9</f>
+        <v>2.0371832715762601E-2</v>
+      </c>
+      <c r="AC9">
+        <f>N9*AB$12*F9+G9*Z$12</f>
+        <v>0.13107936507936507</v>
+      </c>
+      <c r="AD9" s="6">
+        <f>AC9/E9</f>
+        <v>1.7477248677248678</v>
+      </c>
+      <c r="AF9">
+        <f t="shared" si="2"/>
+        <v>8.9782134618554429E-2</v>
+      </c>
+      <c r="AG9" s="6">
+        <f>AF9/E9</f>
+        <v>1.1970951282473925</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33">
+      <c r="A10" t="s">
         <v>64</v>
       </c>
-      <c r="B9">
-        <v>0.2</v>
-      </c>
-      <c r="C9">
+      <c r="C10">
+        <v>0.2</v>
+      </c>
+      <c r="D10">
         <v>2.5</v>
       </c>
-      <c r="D9">
+      <c r="E10">
+        <v>0.45</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
         <v>600</v>
       </c>
-      <c r="E9">
-        <v>0.45</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="I10" t="s">
         <v>65</v>
       </c>
-      <c r="I9">
-        <f>2*PI()*(C9/2)*B9</f>
+      <c r="L10">
+        <f>2*PI()*(D10/2)*C10</f>
         <v>1.5707963267948966</v>
       </c>
-      <c r="J9">
-        <f>E9/I9</f>
+      <c r="M10">
+        <f>E10/L10</f>
         <v>0.28647889756541162</v>
       </c>
-      <c r="L9">
-        <f>PI()*(C9/2)^2</f>
+      <c r="N10">
+        <f>PI()*(D10/2)^2</f>
         <v>4.908738521234052</v>
       </c>
-      <c r="M9">
-        <f>D9/L9</f>
-        <v>122.23099629457562</v>
+      <c r="P10">
+        <f>E10/N10</f>
+        <v>9.1673247220931717E-2</v>
+      </c>
+      <c r="Q10" s="6">
+        <f>P10/P$12</f>
+        <v>1.390387444825895</v>
+      </c>
+      <c r="S10">
+        <f>S$12*D10</f>
+        <v>1000</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="U10" s="6">
+        <f>G10/S10</f>
+        <v>0.6</v>
+      </c>
+      <c r="W10">
+        <f>E10/D10^3</f>
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="X10" s="6">
+        <f>W10/W$12</f>
+        <v>0.72798082684242071</v>
+      </c>
+      <c r="Z10">
+        <f>G10*Z$12</f>
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="AA10">
+        <f>(E10-Z10)/F10</f>
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="AB10">
+        <f>AA10/N10</f>
+        <v>3.972507379573708E-2</v>
+      </c>
+      <c r="AC10">
+        <f>N10*AB$12*F10+G10*Z$12</f>
+        <v>0.48431746031746031</v>
+      </c>
+      <c r="AD10" s="6">
+        <f>AC10/E10</f>
+        <v>1.0762610229276897</v>
+      </c>
+      <c r="AF10">
+        <f t="shared" si="2"/>
+        <v>9.7958537856348088E-2</v>
+      </c>
+      <c r="AG10" s="6">
+        <f>AF10/E10</f>
+        <v>0.21768563968077353</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33">
+      <c r="X11" s="6"/>
+    </row>
+    <row r="12" spans="1:33">
+      <c r="M12">
+        <f>AVERAGE(M3:M9)</f>
+        <v>6.2362342071569425E-2</v>
+      </c>
+      <c r="O12" t="s">
+        <v>158</v>
+      </c>
+      <c r="P12">
+        <f>AVERAGE(P3:P10)</f>
+        <v>6.5933598265777701E-2</v>
+      </c>
+      <c r="Q12" s="6">
+        <f>AVERAGE(Q3:Q10)</f>
+        <v>0.99999999999999978</v>
+      </c>
+      <c r="S12">
+        <f>500/1.25</f>
+        <v>400</v>
+      </c>
+      <c r="T12">
+        <f>10/1.25</f>
+        <v>8</v>
+      </c>
+      <c r="W12">
+        <f>AVERAGE(W3:W10)</f>
+        <v>3.9561481481481475E-2</v>
+      </c>
+      <c r="X12" s="6">
+        <f>AVERAGE(X3:X10)</f>
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="Z12">
+        <v>1E-4</v>
+      </c>
+      <c r="AB12">
+        <f>AVERAGE(AB3:AB10)</f>
+        <v>4.3220621599822692E-2</v>
+      </c>
+      <c r="AD12" s="7">
+        <f>AVERAGE(AD3:AD10)</f>
+        <v>1.1388370811287478</v>
+      </c>
+      <c r="AG12" s="6">
+        <f>AVERAGE(AG3:AG10)</f>
+        <v>0.90754881606827631</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33">
+      <c r="O13" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q13">
+        <f>STDEV(Q3:Q10)</f>
+        <v>0.26956746896639638</v>
+      </c>
+      <c r="X13">
+        <f>STDEV(X3:X10)</f>
+        <v>0.59948553233565693</v>
+      </c>
+      <c r="AD13">
+        <f>STDEV(AD3:AD10)</f>
+        <v>0.45165968476742585</v>
+      </c>
+      <c r="AG13">
+        <f>STDEV(AG3:AG10)</f>
+        <v>0.3401797404083729</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33">
+      <c r="O15" t="s">
+        <v>68</v>
+      </c>
+      <c r="P15">
+        <f>P12/0.2</f>
+        <v>0.32966799132888847</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3428,19 +4240,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="C1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="K1" s="6" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="K1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="6"/>
+      <c r="L1" s="8"/>
     </row>
     <row r="2" spans="1:19">
       <c r="B2" t="s">
@@ -3492,7 +4304,7 @@
         <v>6</v>
       </c>
       <c r="S2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -3951,7 +4763,7 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B17" s="5">
         <v>3.75</v>

</xml_diff>

<commit_message>
Not sure if I actually tweaked much.
</commit_message>
<xml_diff>
--- a/Source/CalcsAndModels/StockParts.xlsx
+++ b/Source/CalcsAndModels/StockParts.xlsx
@@ -228,7 +228,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="169">
   <si>
     <t>dia</t>
   </si>
@@ -732,6 +732,9 @@
   </si>
   <si>
     <t>heatFactor</t>
+  </si>
+  <si>
+    <t>thrust1m</t>
   </si>
 </sst>
 </file>
@@ -1205,10 +1208,10 @@
   <dimension ref="A1:AB46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y38" sqref="Y38:Y41"/>
+      <selection pane="bottomRight" activeCell="W40" sqref="W40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2776,6 +2779,9 @@
       <c r="V37" t="s">
         <v>81</v>
       </c>
+      <c r="W37" t="s">
+        <v>168</v>
+      </c>
       <c r="Y37" t="s">
         <v>167</v>
       </c>
@@ -2840,6 +2846,10 @@
         <f>G38/$T38</f>
         <v>147.01672609875348</v>
       </c>
+      <c r="W38">
+        <f>P38/C38^2</f>
+        <v>160</v>
+      </c>
       <c r="X38">
         <f>SUM(G38:H38)/E38</f>
         <v>866</v>
@@ -2914,16 +2924,20 @@
         <f>G39/$T39</f>
         <v>97.555255258581482</v>
       </c>
+      <c r="W39">
+        <f t="shared" ref="W39:W41" si="8">P39/C39^2</f>
+        <v>201.6</v>
+      </c>
       <c r="X39">
         <f>SUM(G39:H39)/E39</f>
         <v>566.66666666666663</v>
       </c>
       <c r="Y39">
-        <f t="shared" ref="Y39:Y41" si="8">(Q39*(1+E39))/P39^(1/2)</f>
+        <f t="shared" ref="Y39:Y41" si="9">(Q39*(1+E39))/P39^(1/2)</f>
         <v>56.3436169819011</v>
       </c>
       <c r="Z39">
-        <f t="shared" ref="Z39:Z41" si="9">P39/F39</f>
+        <f t="shared" ref="Z39:Z41" si="10">P39/F39</f>
         <v>40</v>
       </c>
       <c r="AA39">
@@ -3000,16 +3014,20 @@
         <f>G40/$T40</f>
         <v>136.72370950176244</v>
       </c>
+      <c r="W40">
+        <f t="shared" si="8"/>
+        <v>416</v>
+      </c>
       <c r="X40">
         <f>SUM(G40:H40)/E40</f>
         <v>833.33333333333337</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>62.757163244218887</v>
       </c>
       <c r="Z40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>29.885057471264368</v>
       </c>
       <c r="AA40">
@@ -3074,16 +3092,20 @@
         <f>G41/$T41</f>
         <v>905.41478736722684</v>
       </c>
+      <c r="W41">
+        <f t="shared" si="8"/>
+        <v>800</v>
+      </c>
       <c r="X41">
         <f>SUM(G41:H41)/E41</f>
         <v>640</v>
       </c>
       <c r="Y41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>131.25669625775291</v>
       </c>
       <c r="Z41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>248.27586206896552</v>
       </c>
       <c r="AA41">
@@ -3187,7 +3209,7 @@
         <v>1600</v>
       </c>
       <c r="AB44">
-        <f t="shared" ref="AB44:AB46" si="10">N44/E44</f>
+        <f t="shared" ref="AB44:AB46" si="11">N44/E44</f>
         <v>0</v>
       </c>
     </row>
@@ -3205,7 +3227,7 @@
         <v>0.46875</v>
       </c>
       <c r="F45">
-        <f t="shared" ref="F45:F46" si="11">E45+G45*0.0075</f>
+        <f t="shared" ref="F45:F46" si="12">E45+G45*0.0075</f>
         <v>27.326249999999998</v>
       </c>
       <c r="G45" s="1">
@@ -3253,7 +3275,7 @@
         <v>16.222249999999999</v>
       </c>
       <c r="Z45">
-        <f t="shared" ref="Z45:Z46" si="12">P45/F45</f>
+        <f t="shared" ref="Z45:Z46" si="13">P45/F45</f>
         <v>11.527377521613834</v>
       </c>
       <c r="AA45">
@@ -3261,7 +3283,7 @@
         <v>672</v>
       </c>
       <c r="AB45">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -3279,7 +3301,7 @@
         <v>3.90625E-3</v>
       </c>
       <c r="F46">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.25890625</v>
       </c>
       <c r="G46" s="1">
@@ -3327,7 +3349,7 @@
         <v>7.9110243055555554</v>
       </c>
       <c r="Z46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>69.523234761617374</v>
       </c>
       <c r="AA46">
@@ -3335,7 +3357,7 @@
         <v>4608</v>
       </c>
       <c r="AB46">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed techRequired and techObsolete for shapes
I suspect this might be controversial :)
</commit_message>
<xml_diff>
--- a/Source/CalcsAndModels/StockParts.xlsx
+++ b/Source/CalcsAndModels/StockParts.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="4080" windowWidth="30840" windowHeight="18975"/>
+    <workbookView xWindow="3765" yWindow="4080" windowWidth="30840" windowHeight="18975" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tanks" sheetId="3" r:id="rId1"/>
     <sheet name="Decouplers" sheetId="4" r:id="rId2"/>
     <sheet name="Structural" sheetId="5" r:id="rId3"/>
+    <sheet name="Electrics" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_p0">#REF!</definedName>
@@ -228,7 +229,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="202">
   <si>
     <t>dia</t>
   </si>
@@ -762,6 +763,78 @@
   </si>
   <si>
     <t>RF Vol</t>
+  </si>
+  <si>
+    <t>Batteries</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Z-1k</t>
+  </si>
+  <si>
+    <t>batteryBank</t>
+  </si>
+  <si>
+    <t>Dia</t>
+  </si>
+  <si>
+    <t>largeElectrics</t>
+  </si>
+  <si>
+    <t>Charge</t>
+  </si>
+  <si>
+    <t>batteryBankLarge</t>
+  </si>
+  <si>
+    <t>specializedElectrics</t>
+  </si>
+  <si>
+    <t>Z-200</t>
+  </si>
+  <si>
+    <t>Z-4k</t>
+  </si>
+  <si>
+    <t>batteryBankMini</t>
+  </si>
+  <si>
+    <t>electrics</t>
+  </si>
+  <si>
+    <t>Z-100</t>
+  </si>
+  <si>
+    <t>batteryPack</t>
+  </si>
+  <si>
+    <t>scienceTech</t>
+  </si>
+  <si>
+    <t>Z-400</t>
+  </si>
+  <si>
+    <t>ksp_r_largeBatteryPack</t>
+  </si>
+  <si>
+    <t>advElectrics</t>
+  </si>
+  <si>
+    <t>Unit/mass</t>
+  </si>
+  <si>
+    <t>RTG</t>
+  </si>
+  <si>
+    <t>PB-NUK</t>
+  </si>
+  <si>
+    <t>rtg</t>
   </si>
 </sst>
 </file>
@@ -900,7 +973,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -910,6 +983,9 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="25" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1234,7 +1310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -1252,15 +1328,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="N1" s="9" t="s">
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="N1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="9"/>
+      <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:30">
       <c r="B2" t="s">
@@ -3499,7 +3575,7 @@
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4373,7 +4449,7 @@
   <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection sqref="A1:R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -4386,19 +4462,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="G1" s="9" t="s">
+      <c r="C1" s="10"/>
+      <c r="G1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="K1" s="9" t="s">
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="K1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="L1" s="9"/>
+      <c r="L1" s="10"/>
     </row>
     <row r="2" spans="1:19">
       <c r="B2" t="s">
@@ -5482,4 +5558,381 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="9"/>
+      <c r="G1" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M2" t="s">
+        <v>185</v>
+      </c>
+      <c r="O2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4">
+        <v>1.25</v>
+      </c>
+      <c r="E4">
+        <f>0.1108553*2</f>
+        <v>0.22171060000000001</v>
+      </c>
+      <c r="F4">
+        <v>0.05</v>
+      </c>
+      <c r="G4">
+        <v>0.2</v>
+      </c>
+      <c r="H4">
+        <v>0.2</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <v>3200</v>
+      </c>
+      <c r="M4">
+        <v>1000</v>
+      </c>
+      <c r="O4">
+        <f>PI()*(D4/2)^2*E4</f>
+        <v>0.27207984069647861</v>
+      </c>
+      <c r="P4">
+        <f>F4/O4</f>
+        <v>0.18376958716238739</v>
+      </c>
+      <c r="Q4">
+        <f>M4/F4</f>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5">
+        <v>2.5</v>
+      </c>
+      <c r="E5">
+        <v>0.25</v>
+      </c>
+      <c r="F5">
+        <v>0.2</v>
+      </c>
+      <c r="G5">
+        <v>0.2</v>
+      </c>
+      <c r="H5">
+        <v>0.2</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>8</v>
+      </c>
+      <c r="K5">
+        <v>3200</v>
+      </c>
+      <c r="M5">
+        <v>4000</v>
+      </c>
+      <c r="O5">
+        <f>PI()*(D5/2)^2*E5</f>
+        <v>1.227184630308513</v>
+      </c>
+      <c r="P5">
+        <f>F5/O5</f>
+        <v>0.16297466172610084</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ref="Q5:Q9" si="0">M5/F5</f>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6">
+        <v>0.625</v>
+      </c>
+      <c r="E6">
+        <v>0.2</v>
+      </c>
+      <c r="F6">
+        <v>0.01</v>
+      </c>
+      <c r="G6">
+        <v>0.2</v>
+      </c>
+      <c r="H6">
+        <v>0.2</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>8</v>
+      </c>
+      <c r="K6">
+        <v>3200</v>
+      </c>
+      <c r="M6">
+        <v>200</v>
+      </c>
+      <c r="O6">
+        <f>PI()*(D6/2)^2*E6</f>
+        <v>6.1359231515425654E-2</v>
+      </c>
+      <c r="P6">
+        <f>F6/O6</f>
+        <v>0.16297466172610081</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" t="s">
+        <v>194</v>
+      </c>
+      <c r="F8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G8">
+        <v>0.2</v>
+      </c>
+      <c r="H8">
+        <v>0.2</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>8</v>
+      </c>
+      <c r="K8">
+        <v>3200</v>
+      </c>
+      <c r="M8">
+        <v>100</v>
+      </c>
+      <c r="O8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="P8">
+        <f t="shared" ref="P7:P9" si="1">F8/O8</f>
+        <v>1.25</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" t="s">
+        <v>197</v>
+      </c>
+      <c r="F9">
+        <v>0.02</v>
+      </c>
+      <c r="G9">
+        <v>0.2</v>
+      </c>
+      <c r="H9">
+        <v>0.2</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>3200</v>
+      </c>
+      <c r="M9">
+        <v>400</v>
+      </c>
+      <c r="O9">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>0.46511627906976749</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12" t="s">
+        <v>201</v>
+      </c>
+      <c r="C12" t="s">
+        <v>187</v>
+      </c>
+      <c r="D12">
+        <v>0.2</v>
+      </c>
+      <c r="E12">
+        <f>0.3268025*2</f>
+        <v>0.65360499999999999</v>
+      </c>
+      <c r="F12">
+        <v>0.08</v>
+      </c>
+      <c r="G12">
+        <v>0.2</v>
+      </c>
+      <c r="H12">
+        <v>0.2</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>7</v>
+      </c>
+      <c r="K12">
+        <v>3000</v>
+      </c>
+      <c r="M12">
+        <v>0.75</v>
+      </c>
+      <c r="O12">
+        <f>PI()*(D12/2)^2*E12</f>
+        <v>2.053360666349557E-2</v>
+      </c>
+      <c r="P12">
+        <f>F12/O12</f>
+        <v>3.8960520336752706</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" ref="Q12" si="2">M12/F12</f>
+        <v>9.375</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>